<commit_message>
edit actual output (missing value)
</commit_message>
<xml_diff>
--- a/Indonesia_indicator/test_case.xlsx
+++ b/Indonesia_indicator/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QA-practice\Indonesia_indicator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5717159E-11CA-421B-AF5E-D65E56B80648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3073FC49-DB29-407F-824F-6DE48DEB5A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{B88F0274-8152-4EBC-A351-10C41F17EBC4}"/>
+    <workbookView xWindow="615" yWindow="1845" windowWidth="18405" windowHeight="10320" xr2:uid="{B88F0274-8152-4EBC-A351-10C41F17EBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Feature</t>
   </si>
@@ -324,9 +324,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -346,6 +343,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,20 +663,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F55ECE6-69BA-4769-B702-57B8476DBFD1}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="27.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="27.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -706,346 +706,348 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="2"/>
+      <c r="H17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>